<commit_message>
Ship Resistance using ITTC
</commit_message>
<xml_diff>
--- a/Table.xlsx
+++ b/Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\Documents\GitHub\ResistanceTestExtrapolation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EA7D0B-B78B-418F-B3F3-42CE0AABA5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82313E5E-D7D1-4557-AC15-3C413739937F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{7D64D09A-60FA-43C1-B1C5-0E2F41180447}"/>
+    <workbookView xWindow="-10044" yWindow="576" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{7D64D09A-60FA-43C1-B1C5-0E2F41180447}"/>
   </bookViews>
   <sheets>
     <sheet name="Table9" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Table 12" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1741,7 +1740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA634AD3-67C5-4C7B-97B0-3D52B9D0B3F9}">
   <dimension ref="B2:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
@@ -1774,7 +1773,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D19" si="0">$B$2*C3</f>
+        <f t="shared" ref="D3:D10" si="0">$B$2*C3</f>
         <v>200000</v>
       </c>
       <c r="E3">

</xml_diff>